<commit_message>
refactor(ui): Aplica paleta de colores Q-Vision y rediseña vistas 'base' y 'analysis'
</commit_message>
<xml_diff>
--- a/backend/uploads/plantilla_maestra.xlsx
+++ b/backend/uploads/plantilla_maestra.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesus\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/edf58a523d585a4a/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70BC9050-E9DE-4EC6-9FA2-0E313012E5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{579FF7D6-1145-45E2-9B2A-1B68B78B9E82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85F07528-6FDF-4390-B3A4-2F8FF6ADE32F}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,22 +23,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>{{ID_CASO}}</t>
   </si>
   <si>
-    <t>{{TITULO_CASO}}</t>
-  </si>
-  <si>
-    <t>{{PASOS_PRUEBA}}</t>
+    <t>{{TITULO}}</t>
+  </si>
+  <si>
+    <t>{{DESCRIPCION}}</t>
+  </si>
+  <si>
+    <t>{{MODULO}}</t>
+  </si>
+  <si>
+    <t>{{ID_REQUISITO}}</t>
+  </si>
+  <si>
+    <t>{{HISTORIA_USUARIO}}</t>
+  </si>
+  <si>
+    <t>{{PRECONDICIONES}}</t>
+  </si>
+  <si>
+    <t>{{PASOS_EJECUCION}}</t>
+  </si>
+  <si>
+    <t>{{DATOS_PRUEBA}}</t>
+  </si>
+  <si>
+    <t>{{RESULTADO_ESPERADO}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -51,12 +72,6 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF444746"/>
-      <name val="Google Sans Text"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -66,7 +81,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -74,31 +89,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -317,33 +314,73 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A8:R8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27" thickBot="1">
-      <c r="A1" s="2" t="s">
+    <row r="8" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" ht="13.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -356,7 +393,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -368,7 +405,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -382,7 +419,7 @@
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>